<commit_message>
fin de  20 AGOSTO
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 07  JULIO  2021/BALANCE ABASTOS   J U L I O        2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 07  JULIO  2021/BALANCE ABASTOS   J U L I O        2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20340" windowHeight="10725" firstSheet="10" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20340" windowHeight="10725" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="E N E R O     2 0 2 1    " sheetId="1" r:id="rId1"/>
@@ -5511,31 +5511,29 @@
     <xf numFmtId="44" fontId="7" fillId="19" borderId="81" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="7" fillId="19" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="7" fillId="19" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="44" fontId="54" fillId="4" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="57" fillId="4" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="16" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="14" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5577,26 +5575,31 @@
     <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="15" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5611,14 +5614,14 @@
     <xf numFmtId="166" fontId="6" fillId="15" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="14" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="35" fillId="10" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5637,6 +5640,15 @@
     </xf>
     <xf numFmtId="44" fontId="35" fillId="10" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="35" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="16" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -5716,26 +5728,32 @@
     <xf numFmtId="44" fontId="49" fillId="0" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="35" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="53" fillId="8" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="53" fillId="8" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="44" fontId="53" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="44" fontId="53" fillId="8" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="16" fillId="8" borderId="67" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5776,32 +5794,17 @@
     <xf numFmtId="44" fontId="16" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="8" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="16" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="8" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="8" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="53" fillId="8" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="53" fillId="8" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="53" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="53" fillId="8" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5812,9 +5815,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="54" fillId="4" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="57" fillId="4" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="16" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -10927,17 +10927,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="506" t="s">
+      <c r="C1" s="487" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="506"/>
-      <c r="E1" s="506"/>
-      <c r="F1" s="506"/>
-      <c r="G1" s="506"/>
-      <c r="H1" s="506"/>
-      <c r="I1" s="506"/>
-      <c r="J1" s="506"/>
-      <c r="K1" s="506"/>
+      <c r="D1" s="487"/>
+      <c r="E1" s="487"/>
+      <c r="F1" s="487"/>
+      <c r="G1" s="487"/>
+      <c r="H1" s="487"/>
+      <c r="I1" s="487"/>
+      <c r="J1" s="487"/>
+      <c r="K1" s="487"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -10968,17 +10968,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="507" t="s">
+      <c r="B3" s="488" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="508"/>
+      <c r="C3" s="489"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="509" t="s">
+      <c r="H3" s="490" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="509"/>
+      <c r="I3" s="490"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -11007,14 +11007,14 @@
       <c r="D4" s="23">
         <v>44201</v>
       </c>
-      <c r="E4" s="510" t="s">
+      <c r="E4" s="491" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="511"/>
-      <c r="H4" s="512" t="s">
+      <c r="F4" s="492"/>
+      <c r="H4" s="493" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="513"/>
+      <c r="I4" s="494"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -13625,61 +13625,61 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="493" t="s">
+      <c r="H64" s="495" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="494"/>
+      <c r="I64" s="496"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="495">
+      <c r="K64" s="497">
         <f>I62+L62</f>
         <v>360753.85</v>
       </c>
-      <c r="L64" s="496"/>
-      <c r="M64" s="497">
+      <c r="L64" s="498"/>
+      <c r="M64" s="499">
         <f>M62+N62</f>
         <v>2886514.7</v>
       </c>
-      <c r="N64" s="498"/>
+      <c r="N64" s="500"/>
       <c r="O64" s="102"/>
       <c r="P64" s="99"/>
       <c r="Q64" s="99"/>
       <c r="S64" s="174"/>
     </row>
     <row r="65" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="505" t="s">
+      <c r="D65" s="507" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="505"/>
+      <c r="E65" s="507"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>2365880.5699999998</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="484">
+      <c r="P65" s="508">
         <f>P62+Q62</f>
         <v>3321521.28</v>
       </c>
-      <c r="Q65" s="485"/>
+      <c r="Q65" s="509"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="486" t="s">
+      <c r="D66" s="510" t="s">
         <v>18</v>
       </c>
-      <c r="E66" s="486"/>
+      <c r="E66" s="510"/>
       <c r="F66" s="95">
         <v>-2276696.6800000002</v>
       </c>
-      <c r="I66" s="487" t="s">
+      <c r="I66" s="511" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="488"/>
-      <c r="K66" s="489">
+      <c r="J66" s="512"/>
+      <c r="K66" s="513">
         <f>F68+F69+F70</f>
         <v>344253.98999999964</v>
       </c>
-      <c r="L66" s="490"/>
+      <c r="L66" s="514"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
@@ -13713,11 +13713,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="491">
+      <c r="K68" s="515">
         <f>-C4</f>
         <v>-250864.68</v>
       </c>
-      <c r="L68" s="492"/>
+      <c r="L68" s="516"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -13741,22 +13741,22 @@
       <c r="C70" s="119">
         <v>44230</v>
       </c>
-      <c r="D70" s="499" t="s">
+      <c r="D70" s="501" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="500"/>
+      <c r="E70" s="502"/>
       <c r="F70" s="120">
         <v>209541.1</v>
       </c>
-      <c r="I70" s="501" t="s">
+      <c r="I70" s="503" t="s">
         <v>25</v>
       </c>
-      <c r="J70" s="502"/>
-      <c r="K70" s="503">
+      <c r="J70" s="504"/>
+      <c r="K70" s="505">
         <f>K66+K68</f>
         <v>93389.309999999648</v>
       </c>
-      <c r="L70" s="504"/>
+      <c r="L70" s="506"/>
       <c r="P70" s="50"/>
       <c r="Q70" s="7"/>
       <c r="S70" s="121"/>
@@ -13860,11 +13860,11 @@
     <sortCondition ref="J35:J54"/>
   </sortState>
   <mergeCells count="17">
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="P65:Q65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="K68:L68"/>
     <mergeCell ref="H64:I64"/>
     <mergeCell ref="K64:L64"/>
     <mergeCell ref="M64:N64"/>
@@ -13872,11 +13872,11 @@
     <mergeCell ref="I70:J70"/>
     <mergeCell ref="K70:L70"/>
     <mergeCell ref="D65:E65"/>
-    <mergeCell ref="P65:Q65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <phoneticPr fontId="41" type="noConversion"/>
   <pageMargins left="0.2" right="0.16" top="0.34" bottom="0.32" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -15265,7 +15265,7 @@
   </sheetPr>
   <dimension ref="A1:AG92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F11" workbookViewId="0">
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
@@ -15301,20 +15301,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="554" t="s">
+      <c r="B1" s="530" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="506" t="s">
+      <c r="C1" s="487" t="s">
         <v>503</v>
       </c>
-      <c r="D1" s="506"/>
-      <c r="E1" s="506"/>
-      <c r="F1" s="506"/>
-      <c r="G1" s="506"/>
-      <c r="H1" s="506"/>
-      <c r="I1" s="506"/>
-      <c r="J1" s="506"/>
-      <c r="K1" s="506"/>
+      <c r="D1" s="487"/>
+      <c r="E1" s="487"/>
+      <c r="F1" s="487"/>
+      <c r="G1" s="487"/>
+      <c r="H1" s="487"/>
+      <c r="I1" s="487"/>
+      <c r="J1" s="487"/>
+      <c r="K1" s="487"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -15324,7 +15324,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="555"/>
+      <c r="B2" s="531"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -15343,27 +15343,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="537" t="s">
+      <c r="AB2" s="543" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="537"/>
-      <c r="AD2" s="537"/>
-      <c r="AE2" s="537"/>
-      <c r="AF2" s="537"/>
-      <c r="AG2" s="537"/>
+      <c r="AC2" s="543"/>
+      <c r="AD2" s="543"/>
+      <c r="AE2" s="543"/>
+      <c r="AF2" s="543"/>
+      <c r="AG2" s="543"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="507" t="s">
+      <c r="B3" s="488" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="508"/>
+      <c r="C3" s="489"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="509" t="s">
+      <c r="H3" s="490" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="509"/>
+      <c r="I3" s="490"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -15371,7 +15371,7 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="P3" s="527" t="s">
+      <c r="P3" s="533" t="s">
         <v>562</v>
       </c>
       <c r="Q3" s="393"/>
@@ -15384,12 +15384,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="537"/>
-      <c r="AC3" s="537"/>
-      <c r="AD3" s="537"/>
-      <c r="AE3" s="537"/>
-      <c r="AF3" s="537"/>
-      <c r="AG3" s="537"/>
+      <c r="AB3" s="543"/>
+      <c r="AC3" s="543"/>
+      <c r="AD3" s="543"/>
+      <c r="AE3" s="543"/>
+      <c r="AF3" s="543"/>
+      <c r="AG3" s="543"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -15402,14 +15402,14 @@
       <c r="D4" s="23">
         <v>44353</v>
       </c>
-      <c r="E4" s="510" t="s">
+      <c r="E4" s="491" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="511"/>
-      <c r="H4" s="512" t="s">
+      <c r="F4" s="492"/>
+      <c r="H4" s="493" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="513"/>
+      <c r="I4" s="494"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -15420,7 +15420,7 @@
         <v>10</v>
       </c>
       <c r="O4" s="365"/>
-      <c r="P4" s="527"/>
+      <c r="P4" s="533"/>
       <c r="Q4" s="393"/>
       <c r="R4" s="30"/>
       <c r="S4" s="31"/>
@@ -15435,16 +15435,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="538" t="s">
+      <c r="AB4" s="544" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="539"/>
+      <c r="AC4" s="545"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="540" t="s">
+      <c r="AE4" s="546" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="540"/>
-      <c r="AG4" s="540"/>
+      <c r="AF4" s="546"/>
+      <c r="AG4" s="546"/>
     </row>
     <row r="5" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
@@ -16856,10 +16856,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="545" t="s">
+      <c r="AE23" s="551" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="546"/>
+      <c r="AF23" s="552"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -17003,11 +17003,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="547" t="s">
+      <c r="AE25" s="553" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="548"/>
-      <c r="AG25" s="551">
+      <c r="AF25" s="554"/>
+      <c r="AG25" s="557">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -17078,9 +17078,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="549"/>
-      <c r="AF26" s="550"/>
-      <c r="AG26" s="552"/>
+      <c r="AE26" s="555"/>
+      <c r="AF26" s="556"/>
+      <c r="AG26" s="558"/>
     </row>
     <row r="27" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="34"/>
@@ -17255,10 +17255,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="541" t="s">
+      <c r="AB29" s="547" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="543">
+      <c r="AC29" s="549">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -17294,11 +17294,11 @@
         <v>0</v>
       </c>
       <c r="O30" s="7"/>
-      <c r="P30" s="528">
+      <c r="P30" s="534">
         <f>SUM(P5:P29)</f>
         <v>-163726</v>
       </c>
-      <c r="Q30" s="528"/>
+      <c r="Q30" s="534"/>
       <c r="R30" s="7">
         <v>0</v>
       </c>
@@ -17312,8 +17312,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="542"/>
-      <c r="AC30" s="544"/>
+      <c r="AB30" s="548"/>
+      <c r="AC30" s="550"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -18675,21 +18675,21 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="493" t="s">
+      <c r="H64" s="495" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="494"/>
+      <c r="I64" s="496"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="495">
+      <c r="K64" s="497">
         <f>I62+L62</f>
         <v>339830.06000000006</v>
       </c>
-      <c r="L64" s="496"/>
-      <c r="M64" s="497">
+      <c r="L64" s="498"/>
+      <c r="M64" s="499">
         <f>M62+N62</f>
         <v>2936130</v>
       </c>
-      <c r="N64" s="498"/>
+      <c r="N64" s="500"/>
       <c r="O64" s="367"/>
       <c r="P64" s="367"/>
       <c r="Q64" s="367"/>
@@ -18704,40 +18704,40 @@
       <c r="AG64" s="327"/>
     </row>
     <row r="65" spans="2:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="505" t="s">
+      <c r="D65" s="507" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="505"/>
+      <c r="E65" s="507"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>2702101.7199999997</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="R65" s="484">
+      <c r="R65" s="508">
         <f>R62+S62</f>
         <v>3138957.44</v>
       </c>
-      <c r="S65" s="485"/>
+      <c r="S65" s="509"/>
       <c r="U65" s="50"/>
     </row>
     <row r="66" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="486" t="s">
+      <c r="D66" s="510" t="s">
         <v>502</v>
       </c>
-      <c r="E66" s="486"/>
+      <c r="E66" s="510"/>
       <c r="F66" s="95">
         <v>-2720820.95</v>
       </c>
-      <c r="I66" s="487" t="s">
+      <c r="I66" s="511" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="488"/>
-      <c r="K66" s="489">
+      <c r="J66" s="512"/>
+      <c r="K66" s="513">
         <f>F68+F69+F70</f>
         <v>381077.48999999953</v>
       </c>
-      <c r="L66" s="490"/>
+      <c r="L66" s="514"/>
       <c r="R66" s="50"/>
       <c r="U66" s="107"/>
     </row>
@@ -18771,11 +18771,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="491">
+      <c r="K68" s="515">
         <f>-C4</f>
         <v>-255764.39</v>
       </c>
-      <c r="L68" s="492"/>
+      <c r="L68" s="516"/>
       <c r="M68" s="116"/>
       <c r="R68" s="50"/>
       <c r="S68" s="7"/>
@@ -18799,22 +18799,22 @@
       <c r="C70" s="119">
         <v>44377</v>
       </c>
-      <c r="D70" s="499" t="s">
+      <c r="D70" s="501" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="500"/>
+      <c r="E70" s="502"/>
       <c r="F70" s="120">
         <v>308642.71999999997</v>
       </c>
-      <c r="I70" s="501" t="s">
+      <c r="I70" s="503" t="s">
         <v>25</v>
       </c>
-      <c r="J70" s="502"/>
-      <c r="K70" s="503">
+      <c r="J70" s="504"/>
+      <c r="K70" s="505">
         <f>K66+K68</f>
         <v>125313.09999999951</v>
       </c>
-      <c r="L70" s="504"/>
+      <c r="L70" s="506"/>
       <c r="R70" s="50"/>
       <c r="S70" s="7"/>
       <c r="U70" s="121"/>
@@ -18830,14 +18830,14 @@
       <c r="S71" s="7"/>
     </row>
     <row r="72" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I72" s="529" t="s">
+      <c r="I72" s="535" t="s">
         <v>610</v>
       </c>
-      <c r="J72" s="530"/>
-      <c r="K72" s="533">
+      <c r="J72" s="536"/>
+      <c r="K72" s="539">
         <v>163726</v>
       </c>
-      <c r="L72" s="534"/>
+      <c r="L72" s="540"/>
       <c r="R72" s="7"/>
       <c r="S72" s="7"/>
     </row>
@@ -18846,10 +18846,10 @@
       <c r="C73" s="128"/>
       <c r="D73" s="129"/>
       <c r="E73" s="7"/>
-      <c r="I73" s="531"/>
-      <c r="J73" s="532"/>
-      <c r="K73" s="535"/>
-      <c r="L73" s="536"/>
+      <c r="I73" s="537"/>
+      <c r="J73" s="538"/>
+      <c r="K73" s="541"/>
+      <c r="L73" s="542"/>
       <c r="M73" s="2"/>
       <c r="N73" s="60"/>
       <c r="O73" s="165"/>
@@ -18901,7 +18901,7 @@
       <c r="C76" s="130"/>
       <c r="E76" s="7"/>
       <c r="M76" s="4"/>
-      <c r="AC76" s="553"/>
+      <c r="AC76" s="532"/>
       <c r="AD76" s="342"/>
       <c r="AE76" s="342"/>
       <c r="AF76" s="342"/>
@@ -18914,7 +18914,7 @@
       <c r="E77" s="7"/>
       <c r="F77" s="273"/>
       <c r="M77" s="4"/>
-      <c r="AC77" s="553"/>
+      <c r="AC77" s="532"/>
       <c r="AD77" s="342"/>
       <c r="AE77" s="342"/>
       <c r="AF77" s="342"/>
@@ -19008,22 +19008,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="AC76:AC77"/>
-    <mergeCell ref="R65:S65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="D65:E65"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="P30:Q30"/>
     <mergeCell ref="I72:J73"/>
@@ -19039,6 +19023,22 @@
     <mergeCell ref="AE23:AF23"/>
     <mergeCell ref="AE25:AF26"/>
     <mergeCell ref="AG25:AG26"/>
+    <mergeCell ref="AC76:AC77"/>
+    <mergeCell ref="R65:S65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.49" right="0.23622047244094491" top="0.47244094488188981" bottom="0.27559055118110237" header="0.70866141732283472" footer="0.31496062992125984"/>
   <pageSetup scale="90" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -20376,25 +20376,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="554" t="s">
+      <c r="B1" s="530" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="506" t="s">
+      <c r="C1" s="487" t="s">
         <v>503</v>
       </c>
-      <c r="D1" s="506"/>
-      <c r="E1" s="506"/>
-      <c r="F1" s="506"/>
-      <c r="G1" s="506"/>
-      <c r="H1" s="506"/>
-      <c r="I1" s="506"/>
-      <c r="J1" s="506"/>
-      <c r="K1" s="506"/>
+      <c r="D1" s="487"/>
+      <c r="E1" s="487"/>
+      <c r="F1" s="487"/>
+      <c r="G1" s="487"/>
+      <c r="H1" s="487"/>
+      <c r="I1" s="487"/>
+      <c r="J1" s="487"/>
+      <c r="K1" s="487"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="555"/>
+      <c r="B2" s="531"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -20404,27 +20404,27 @@
       <c r="L2" s="12"/>
       <c r="M2" s="3"/>
       <c r="N2" s="6"/>
-      <c r="Q2" s="537" t="s">
+      <c r="Q2" s="543" t="s">
         <v>596</v>
       </c>
-      <c r="R2" s="537"/>
-      <c r="S2" s="537"/>
-      <c r="T2" s="537"/>
-      <c r="U2" s="537"/>
-      <c r="V2" s="537"/>
+      <c r="R2" s="543"/>
+      <c r="S2" s="543"/>
+      <c r="T2" s="543"/>
+      <c r="U2" s="543"/>
+      <c r="V2" s="543"/>
     </row>
     <row r="3" spans="1:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="507" t="s">
+      <c r="B3" s="488" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="508"/>
+      <c r="C3" s="489"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="509" t="s">
+      <c r="H3" s="490" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="509"/>
+      <c r="I3" s="490"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -20432,12 +20432,12 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="Q3" s="537"/>
-      <c r="R3" s="537"/>
-      <c r="S3" s="537"/>
-      <c r="T3" s="537"/>
-      <c r="U3" s="537"/>
-      <c r="V3" s="537"/>
+      <c r="Q3" s="543"/>
+      <c r="R3" s="543"/>
+      <c r="S3" s="543"/>
+      <c r="T3" s="543"/>
+      <c r="U3" s="543"/>
+      <c r="V3" s="543"/>
     </row>
     <row r="4" spans="1:23" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -20450,14 +20450,14 @@
       <c r="D4" s="23">
         <v>44353</v>
       </c>
-      <c r="E4" s="510" t="s">
+      <c r="E4" s="491" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="511"/>
-      <c r="H4" s="512" t="s">
+      <c r="F4" s="492"/>
+      <c r="H4" s="493" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="513"/>
+      <c r="I4" s="494"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -20469,16 +20469,16 @@
       </c>
       <c r="O4" s="365"/>
       <c r="P4" s="29"/>
-      <c r="Q4" s="538" t="s">
+      <c r="Q4" s="544" t="s">
         <v>527</v>
       </c>
-      <c r="R4" s="539"/>
+      <c r="R4" s="545"/>
       <c r="S4" s="99"/>
-      <c r="T4" s="540" t="s">
+      <c r="T4" s="546" t="s">
         <v>567</v>
       </c>
-      <c r="U4" s="540"/>
-      <c r="V4" s="540"/>
+      <c r="U4" s="546"/>
+      <c r="V4" s="546"/>
       <c r="W4" s="99"/>
     </row>
     <row r="5" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -21477,10 +21477,10 @@
         <v>0</v>
       </c>
       <c r="S23" s="99"/>
-      <c r="T23" s="545" t="s">
+      <c r="T23" s="551" t="s">
         <v>564</v>
       </c>
-      <c r="U23" s="546"/>
+      <c r="U23" s="552"/>
       <c r="V23" s="339">
         <f>SUM(V6:V22)</f>
         <v>2323600</v>
@@ -21584,11 +21584,11 @@
         <v>138607</v>
       </c>
       <c r="S25" s="99"/>
-      <c r="T25" s="547" t="s">
+      <c r="T25" s="553" t="s">
         <v>565</v>
       </c>
-      <c r="U25" s="548"/>
-      <c r="V25" s="551">
+      <c r="U25" s="554"/>
+      <c r="V25" s="557">
         <f>R29-V23</f>
         <v>163726</v>
       </c>
@@ -21637,9 +21637,9 @@
         <v>107480</v>
       </c>
       <c r="S26" s="99"/>
-      <c r="T26" s="549"/>
-      <c r="U26" s="550"/>
-      <c r="V26" s="552"/>
+      <c r="T26" s="555"/>
+      <c r="U26" s="556"/>
+      <c r="V26" s="558"/>
       <c r="W26" s="99"/>
     </row>
     <row r="27" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -21762,10 +21762,10 @@
       </c>
       <c r="O29" s="7"/>
       <c r="P29" s="29"/>
-      <c r="Q29" s="541" t="s">
+      <c r="Q29" s="547" t="s">
         <v>562</v>
       </c>
-      <c r="R29" s="543">
+      <c r="R29" s="549">
         <f>SUM(R5:R28)</f>
         <v>2487326</v>
       </c>
@@ -21802,8 +21802,8 @@
       </c>
       <c r="O30" s="7"/>
       <c r="P30" s="373"/>
-      <c r="Q30" s="542"/>
-      <c r="R30" s="544"/>
+      <c r="Q30" s="548"/>
+      <c r="R30" s="550"/>
       <c r="S30" s="99"/>
       <c r="T30" s="99"/>
       <c r="U30" s="99"/>
@@ -22428,21 +22428,21 @@
       <c r="A50" s="60"/>
       <c r="B50" s="100"/>
       <c r="C50" s="4"/>
-      <c r="H50" s="493" t="s">
+      <c r="H50" s="495" t="s">
         <v>16</v>
       </c>
-      <c r="I50" s="494"/>
+      <c r="I50" s="496"/>
       <c r="J50" s="101"/>
-      <c r="K50" s="495">
+      <c r="K50" s="497">
         <f>I48+L48</f>
         <v>339830.06000000006</v>
       </c>
-      <c r="L50" s="496"/>
-      <c r="M50" s="497">
+      <c r="L50" s="498"/>
+      <c r="M50" s="499">
         <f>M48+N48</f>
         <v>612530</v>
       </c>
-      <c r="N50" s="498"/>
+      <c r="N50" s="500"/>
       <c r="O50" s="367"/>
       <c r="P50" s="102"/>
       <c r="Q50" s="320"/>
@@ -22454,10 +22454,10 @@
       <c r="W50" s="327"/>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D51" s="505" t="s">
+      <c r="D51" s="507" t="s">
         <v>17</v>
       </c>
-      <c r="E51" s="505"/>
+      <c r="E51" s="507"/>
       <c r="F51" s="103">
         <f>F48-K50-C48</f>
         <v>2702101.7199999997</v>
@@ -22466,22 +22466,22 @@
       <c r="J51" s="105"/>
     </row>
     <row r="52" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D52" s="486" t="s">
+      <c r="D52" s="510" t="s">
         <v>502</v>
       </c>
-      <c r="E52" s="486"/>
+      <c r="E52" s="510"/>
       <c r="F52" s="95">
         <v>-2720820.95</v>
       </c>
-      <c r="I52" s="487" t="s">
+      <c r="I52" s="511" t="s">
         <v>19</v>
       </c>
-      <c r="J52" s="488"/>
-      <c r="K52" s="489">
+      <c r="J52" s="512"/>
+      <c r="K52" s="513">
         <f>F54+F55+F56</f>
         <v>381077.72999999952</v>
       </c>
-      <c r="L52" s="490"/>
+      <c r="L52" s="514"/>
     </row>
     <row r="53" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D53" s="108"/>
@@ -22510,11 +22510,11 @@
         <v>21</v>
       </c>
       <c r="J54" s="115"/>
-      <c r="K54" s="491">
+      <c r="K54" s="515">
         <f>-C4</f>
         <v>-255764.39</v>
       </c>
-      <c r="L54" s="492"/>
+      <c r="L54" s="516"/>
       <c r="M54" s="116"/>
     </row>
     <row r="55" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -22532,22 +22532,22 @@
       <c r="C56" s="119">
         <v>44377</v>
       </c>
-      <c r="D56" s="499" t="s">
+      <c r="D56" s="501" t="s">
         <v>24</v>
       </c>
-      <c r="E56" s="500"/>
+      <c r="E56" s="502"/>
       <c r="F56" s="120">
         <v>308642.71999999997</v>
       </c>
-      <c r="I56" s="501" t="s">
+      <c r="I56" s="503" t="s">
         <v>25</v>
       </c>
-      <c r="J56" s="502"/>
-      <c r="K56" s="503">
+      <c r="J56" s="504"/>
+      <c r="K56" s="505">
         <f>K52+K54</f>
         <v>125313.3399999995</v>
       </c>
-      <c r="L56" s="504"/>
+      <c r="L56" s="506"/>
     </row>
     <row r="57" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C57" s="122"/>
@@ -22603,7 +22603,7 @@
       <c r="C62" s="130"/>
       <c r="E62" s="7"/>
       <c r="M62" s="4"/>
-      <c r="R62" s="553"/>
+      <c r="R62" s="532"/>
       <c r="S62" s="379"/>
       <c r="T62" s="379"/>
       <c r="U62" s="379"/>
@@ -22616,7 +22616,7 @@
       <c r="E63" s="7"/>
       <c r="F63" s="273"/>
       <c r="M63" s="4"/>
-      <c r="R63" s="553"/>
+      <c r="R63" s="532"/>
       <c r="S63" s="379"/>
       <c r="T63" s="379"/>
       <c r="U63" s="379"/>
@@ -22693,23 +22693,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="Q2:V3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="T4:V4"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="T25:U26"/>
-    <mergeCell ref="V25:V26"/>
-    <mergeCell ref="Q29:Q30"/>
-    <mergeCell ref="R29:R30"/>
     <mergeCell ref="R62:R63"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="D52:E52"/>
@@ -22719,6 +22702,23 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="I56:J56"/>
     <mergeCell ref="K56:L56"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="T25:U26"/>
+    <mergeCell ref="V25:V26"/>
+    <mergeCell ref="Q29:Q30"/>
+    <mergeCell ref="R29:R30"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="Q2:V3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="T4:V4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -22734,7 +22734,7 @@
   <dimension ref="A1:AG97"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="K47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="P58" sqref="P58"/>
@@ -22772,20 +22772,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="554" t="s">
+      <c r="B1" s="530" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="506" t="s">
+      <c r="C1" s="487" t="s">
         <v>503</v>
       </c>
-      <c r="D1" s="506"/>
-      <c r="E1" s="506"/>
-      <c r="F1" s="506"/>
-      <c r="G1" s="506"/>
-      <c r="H1" s="506"/>
-      <c r="I1" s="506"/>
-      <c r="J1" s="506"/>
-      <c r="K1" s="506"/>
+      <c r="D1" s="487"/>
+      <c r="E1" s="487"/>
+      <c r="F1" s="487"/>
+      <c r="G1" s="487"/>
+      <c r="H1" s="487"/>
+      <c r="I1" s="487"/>
+      <c r="J1" s="487"/>
+      <c r="K1" s="487"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -22795,7 +22795,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="555"/>
+      <c r="B2" s="531"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -22814,27 +22814,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="537" t="s">
+      <c r="AB2" s="543" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="537"/>
-      <c r="AD2" s="537"/>
-      <c r="AE2" s="537"/>
-      <c r="AF2" s="537"/>
-      <c r="AG2" s="537"/>
+      <c r="AC2" s="543"/>
+      <c r="AD2" s="543"/>
+      <c r="AE2" s="543"/>
+      <c r="AF2" s="543"/>
+      <c r="AG2" s="543"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="507" t="s">
+      <c r="B3" s="488" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="508"/>
+      <c r="C3" s="489"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="509" t="s">
+      <c r="H3" s="490" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="509"/>
+      <c r="I3" s="490"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -22842,13 +22842,13 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="P3" s="556" t="s">
+      <c r="P3" s="581" t="s">
         <v>663</v>
       </c>
-      <c r="Q3" s="558" t="s">
+      <c r="Q3" s="583" t="s">
         <v>665</v>
       </c>
-      <c r="S3" s="559"/>
+      <c r="S3" s="584"/>
       <c r="W3" s="213" t="s">
         <v>54</v>
       </c>
@@ -22858,12 +22858,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="537"/>
-      <c r="AC3" s="537"/>
-      <c r="AD3" s="537"/>
-      <c r="AE3" s="537"/>
-      <c r="AF3" s="537"/>
-      <c r="AG3" s="537"/>
+      <c r="AB3" s="543"/>
+      <c r="AC3" s="543"/>
+      <c r="AD3" s="543"/>
+      <c r="AE3" s="543"/>
+      <c r="AF3" s="543"/>
+      <c r="AG3" s="543"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -22876,14 +22876,14 @@
       <c r="D4" s="23">
         <v>44377</v>
       </c>
-      <c r="E4" s="510" t="s">
+      <c r="E4" s="491" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="511"/>
-      <c r="H4" s="557" t="s">
+      <c r="F4" s="492"/>
+      <c r="H4" s="582" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="513"/>
+      <c r="I4" s="494"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -22894,10 +22894,10 @@
         <v>10</v>
       </c>
       <c r="O4" s="365"/>
-      <c r="P4" s="556"/>
-      <c r="Q4" s="558"/>
+      <c r="P4" s="581"/>
+      <c r="Q4" s="583"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="559"/>
+      <c r="S4" s="584"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
       <c r="W4" s="213" t="s">
@@ -22909,16 +22909,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="538" t="s">
+      <c r="AB4" s="544" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="539"/>
+      <c r="AC4" s="545"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="540" t="s">
+      <c r="AE4" s="546" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="540"/>
-      <c r="AG4" s="540"/>
+      <c r="AF4" s="546"/>
+      <c r="AG4" s="546"/>
     </row>
     <row r="5" spans="1:33" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
@@ -23195,7 +23195,7 @@
       </c>
       <c r="Q8" s="447"/>
       <c r="R8" s="7">
-        <f t="shared" ref="R8:R43" si="1">C8+I8+M8+N8+L8</f>
+        <f t="shared" ref="R8:R38" si="1">C8+I8+M8+N8+L8</f>
         <v>141476.5</v>
       </c>
       <c r="S8" s="201">
@@ -24355,10 +24355,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="545" t="s">
+      <c r="AE23" s="551" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="546"/>
+      <c r="AF23" s="552"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -24490,11 +24490,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="547" t="s">
+      <c r="AE25" s="553" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="548"/>
-      <c r="AG25" s="551">
+      <c r="AF25" s="554"/>
+      <c r="AG25" s="557">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -24563,9 +24563,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="549"/>
-      <c r="AF26" s="550"/>
-      <c r="AG26" s="552"/>
+      <c r="AE26" s="555"/>
+      <c r="AF26" s="556"/>
+      <c r="AG26" s="558"/>
     </row>
     <row r="27" spans="1:33" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34"/>
@@ -24764,10 +24764,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="541" t="s">
+      <c r="AB29" s="547" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="543">
+      <c r="AC29" s="549">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -24830,8 +24830,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="542"/>
-      <c r="AC30" s="544"/>
+      <c r="AB30" s="548"/>
+      <c r="AC30" s="550"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -25218,7 +25218,7 @@
       <c r="J37" s="233"/>
       <c r="K37" s="144"/>
       <c r="L37" s="358"/>
-      <c r="M37" s="585">
+      <c r="M37" s="484">
         <v>52350</v>
       </c>
       <c r="N37" s="456">
@@ -25280,10 +25280,10 @@
       <c r="J38" s="233"/>
       <c r="K38" s="144"/>
       <c r="L38" s="358"/>
-      <c r="M38" s="586">
+      <c r="M38" s="485">
         <v>185490</v>
       </c>
-      <c r="N38" s="587">
+      <c r="N38" s="486">
         <v>24490</v>
       </c>
       <c r="O38" s="7"/>
@@ -25324,11 +25324,11 @@
       <c r="J39" s="233"/>
       <c r="K39" s="361"/>
       <c r="L39" s="357"/>
-      <c r="M39" s="568">
+      <c r="M39" s="576">
         <f>SUM(M5:M38)</f>
         <v>3989872.22</v>
       </c>
-      <c r="N39" s="570">
+      <c r="N39" s="578">
         <f>SUM(N5:N38)</f>
         <v>688820.5</v>
       </c>
@@ -25377,8 +25377,8 @@
         <f>1145.91+398.99+423.94+498.99+398.99</f>
         <v>2866.8199999999997</v>
       </c>
-      <c r="M40" s="569"/>
-      <c r="N40" s="571"/>
+      <c r="M40" s="577"/>
+      <c r="N40" s="579"/>
       <c r="O40" s="7"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
@@ -25571,10 +25571,10 @@
       <c r="L44" s="358">
         <v>73526</v>
       </c>
-      <c r="M44" s="572" t="s">
+      <c r="M44" s="580" t="s">
         <v>567</v>
       </c>
-      <c r="N44" s="572"/>
+      <c r="N44" s="580"/>
       <c r="O44" s="7"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
@@ -26160,7 +26160,7 @@
       <c r="L57" s="458">
         <v>7482</v>
       </c>
-      <c r="M57" s="560">
+      <c r="M57" s="568">
         <f>SUM(M45:M56)</f>
         <v>3316280</v>
       </c>
@@ -26200,7 +26200,7 @@
       <c r="L58" s="458">
         <v>986</v>
       </c>
-      <c r="M58" s="561"/>
+      <c r="M58" s="569"/>
       <c r="N58" s="476"/>
       <c r="O58" s="7"/>
       <c r="P58" s="7"/>
@@ -26275,10 +26275,10 @@
         <f>1033.33+165.33</f>
         <v>1198.6599999999999</v>
       </c>
-      <c r="M60" s="562" t="s">
+      <c r="M60" s="570" t="s">
         <v>721</v>
       </c>
-      <c r="N60" s="563"/>
+      <c r="N60" s="571"/>
       <c r="O60" s="7"/>
       <c r="P60" s="7"/>
       <c r="Q60" s="7"/>
@@ -26351,11 +26351,11 @@
       <c r="L62" s="458">
         <v>22595.71</v>
       </c>
-      <c r="M62" s="564">
+      <c r="M62" s="572">
         <f>M57-M39</f>
         <v>-673592.2200000002</v>
       </c>
-      <c r="N62" s="565"/>
+      <c r="N62" s="573"/>
       <c r="O62" s="7"/>
       <c r="P62" s="7"/>
       <c r="Q62" s="7"/>
@@ -26391,8 +26391,8 @@
       <c r="L63" s="458">
         <v>1064</v>
       </c>
-      <c r="M63" s="566"/>
-      <c r="N63" s="567"/>
+      <c r="M63" s="574"/>
+      <c r="N63" s="575"/>
       <c r="O63" s="7"/>
       <c r="P63" s="7"/>
       <c r="Q63" s="7"/>
@@ -26582,16 +26582,16 @@
       <c r="A69" s="60"/>
       <c r="B69" s="100"/>
       <c r="C69" s="4"/>
-      <c r="H69" s="493" t="s">
+      <c r="H69" s="495" t="s">
         <v>16</v>
       </c>
-      <c r="I69" s="494"/>
+      <c r="I69" s="496"/>
       <c r="J69" s="101"/>
-      <c r="K69" s="495">
+      <c r="K69" s="497">
         <f>I67+L67</f>
         <v>587206.12</v>
       </c>
-      <c r="L69" s="496"/>
+      <c r="L69" s="498"/>
       <c r="M69" s="471"/>
       <c r="N69" s="472"/>
       <c r="O69" s="367"/>
@@ -26608,40 +26608,40 @@
       <c r="AG69" s="327"/>
     </row>
     <row r="70" spans="1:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="505" t="s">
+      <c r="D70" s="507" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="505"/>
+      <c r="E70" s="507"/>
       <c r="F70" s="103">
         <f>F67-K69-C67</f>
         <v>3436910.52</v>
       </c>
       <c r="I70" s="104"/>
       <c r="J70" s="105"/>
-      <c r="R70" s="484">
+      <c r="R70" s="508">
         <f>R67+S67</f>
         <v>10503773.959999999</v>
       </c>
-      <c r="S70" s="485"/>
+      <c r="S70" s="509"/>
       <c r="U70" s="50"/>
     </row>
     <row r="71" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="486" t="s">
+      <c r="D71" s="510" t="s">
         <v>502</v>
       </c>
-      <c r="E71" s="486"/>
+      <c r="E71" s="510"/>
       <c r="F71" s="95">
         <v>-3290264.27</v>
       </c>
-      <c r="I71" s="487" t="s">
+      <c r="I71" s="511" t="s">
         <v>19</v>
       </c>
-      <c r="J71" s="488"/>
-      <c r="K71" s="489">
+      <c r="J71" s="512"/>
+      <c r="K71" s="513">
         <f>F73+F74+F75</f>
         <v>176424.25</v>
       </c>
-      <c r="L71" s="490"/>
+      <c r="L71" s="514"/>
       <c r="R71" s="50"/>
       <c r="U71" s="107"/>
     </row>
@@ -26675,11 +26675,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="115"/>
-      <c r="K73" s="491">
+      <c r="K73" s="515">
         <f>-C4</f>
         <v>-308642.71999999997</v>
       </c>
-      <c r="L73" s="573"/>
+      <c r="L73" s="559"/>
       <c r="R73" s="50"/>
       <c r="S73" s="7"/>
       <c r="U73" s="50"/>
@@ -26700,22 +26700,22 @@
     </row>
     <row r="75" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C75" s="119"/>
-      <c r="D75" s="499" t="s">
+      <c r="D75" s="501" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="500"/>
+      <c r="E75" s="502"/>
       <c r="F75" s="120">
         <v>0</v>
       </c>
-      <c r="I75" s="501" t="s">
+      <c r="I75" s="503" t="s">
         <v>25</v>
       </c>
-      <c r="J75" s="502"/>
-      <c r="K75" s="503">
+      <c r="J75" s="504"/>
+      <c r="K75" s="505">
         <f>K71+K73</f>
         <v>-132218.46999999997</v>
       </c>
-      <c r="L75" s="503"/>
+      <c r="L75" s="505"/>
       <c r="R75" s="50"/>
       <c r="S75" s="7"/>
       <c r="U75" s="121"/>
@@ -26730,14 +26730,14 @@
       <c r="S76" s="7"/>
     </row>
     <row r="77" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I77" s="574" t="s">
+      <c r="I77" s="560" t="s">
         <v>610</v>
       </c>
-      <c r="J77" s="575"/>
-      <c r="K77" s="578">
-        <v>0</v>
-      </c>
-      <c r="L77" s="579"/>
+      <c r="J77" s="561"/>
+      <c r="K77" s="564">
+        <v>0</v>
+      </c>
+      <c r="L77" s="565"/>
       <c r="R77" s="7"/>
       <c r="S77" s="7"/>
     </row>
@@ -26746,10 +26746,10 @@
       <c r="C78" s="128"/>
       <c r="D78" s="129"/>
       <c r="E78" s="7"/>
-      <c r="I78" s="576"/>
-      <c r="J78" s="577"/>
-      <c r="K78" s="580"/>
-      <c r="L78" s="581"/>
+      <c r="I78" s="562"/>
+      <c r="J78" s="563"/>
+      <c r="K78" s="566"/>
+      <c r="L78" s="567"/>
       <c r="M78" s="2"/>
       <c r="N78" s="60"/>
       <c r="O78" s="165"/>
@@ -26801,7 +26801,7 @@
       <c r="C81" s="130"/>
       <c r="E81" s="7"/>
       <c r="M81" s="4"/>
-      <c r="AC81" s="553"/>
+      <c r="AC81" s="532"/>
       <c r="AD81" s="440"/>
       <c r="AE81" s="440"/>
       <c r="AF81" s="440"/>
@@ -26814,7 +26814,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="273"/>
       <c r="M82" s="4"/>
-      <c r="AC82" s="553"/>
+      <c r="AC82" s="532"/>
       <c r="AD82" s="440"/>
       <c r="AE82" s="440"/>
       <c r="AF82" s="440"/>
@@ -26908,13 +26908,21 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="AC81:AC82"/>
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="I77:J78"/>
-    <mergeCell ref="K77:L78"/>
+    <mergeCell ref="AG25:AG26"/>
+    <mergeCell ref="AB29:AB30"/>
+    <mergeCell ref="AC29:AC30"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="AB2:AG3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="S3:S4"/>
     <mergeCell ref="D71:E71"/>
     <mergeCell ref="I71:J71"/>
     <mergeCell ref="K71:L71"/>
@@ -26930,21 +26938,13 @@
     <mergeCell ref="M39:M40"/>
     <mergeCell ref="N39:N40"/>
     <mergeCell ref="M44:N44"/>
-    <mergeCell ref="AG25:AG26"/>
-    <mergeCell ref="AB29:AB30"/>
-    <mergeCell ref="AC29:AC30"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="AB2:AG3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="AC81:AC82"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="I77:J78"/>
+    <mergeCell ref="K77:L78"/>
   </mergeCells>
   <pageMargins left="0.35433070866141736" right="0.27559055118110237" top="0.27559055118110237" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="90" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -26960,7 +26960,7 @@
   </sheetPr>
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
       <selection activeCell="C107" sqref="C106:C107"/>
     </sheetView>
   </sheetViews>
@@ -28615,12 +28615,12 @@
     <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="32"/>
-      <c r="B47" s="582" t="s">
+      <c r="B47" s="585" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="583"/>
-      <c r="D47" s="583"/>
-      <c r="E47" s="584"/>
+      <c r="C47" s="586"/>
+      <c r="D47" s="586"/>
+      <c r="E47" s="587"/>
       <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -29976,17 +29976,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="506" t="s">
+      <c r="C1" s="487" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="506"/>
-      <c r="E1" s="506"/>
-      <c r="F1" s="506"/>
-      <c r="G1" s="506"/>
-      <c r="H1" s="506"/>
-      <c r="I1" s="506"/>
-      <c r="J1" s="506"/>
-      <c r="K1" s="506"/>
+      <c r="D1" s="487"/>
+      <c r="E1" s="487"/>
+      <c r="F1" s="487"/>
+      <c r="G1" s="487"/>
+      <c r="H1" s="487"/>
+      <c r="I1" s="487"/>
+      <c r="J1" s="487"/>
+      <c r="K1" s="487"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -30017,17 +30017,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="507" t="s">
+      <c r="B3" s="488" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="508"/>
+      <c r="C3" s="489"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="509" t="s">
+      <c r="H3" s="490" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="509"/>
+      <c r="I3" s="490"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -30056,14 +30056,14 @@
       <c r="D4" s="23">
         <v>44230</v>
       </c>
-      <c r="E4" s="510" t="s">
+      <c r="E4" s="491" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="511"/>
-      <c r="H4" s="512" t="s">
+      <c r="F4" s="492"/>
+      <c r="H4" s="493" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="513"/>
+      <c r="I4" s="494"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -32602,61 +32602,61 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="493" t="s">
+      <c r="H64" s="495" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="494"/>
+      <c r="I64" s="496"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="495">
+      <c r="K64" s="497">
         <f>I62+L62</f>
         <v>259947.00000000003</v>
       </c>
-      <c r="L64" s="496"/>
-      <c r="M64" s="497">
+      <c r="L64" s="498"/>
+      <c r="M64" s="499">
         <f>M62+N62</f>
         <v>2744320</v>
       </c>
-      <c r="N64" s="498"/>
+      <c r="N64" s="500"/>
       <c r="O64" s="102"/>
       <c r="P64" s="99"/>
       <c r="Q64" s="99"/>
       <c r="S64" s="174"/>
     </row>
     <row r="65" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="505" t="s">
+      <c r="D65" s="507" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="505"/>
+      <c r="E65" s="507"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>2374814.2599999998</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="484">
+      <c r="P65" s="508">
         <f>P62+Q62</f>
         <v>3144691.75</v>
       </c>
-      <c r="Q65" s="485"/>
+      <c r="Q65" s="509"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="486" t="s">
+      <c r="D66" s="510" t="s">
         <v>18</v>
       </c>
-      <c r="E66" s="486"/>
+      <c r="E66" s="510"/>
       <c r="F66" s="95">
         <v>-2261593.1</v>
       </c>
-      <c r="I66" s="487" t="s">
+      <c r="I66" s="511" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="488"/>
-      <c r="K66" s="489">
+      <c r="J66" s="512"/>
+      <c r="K66" s="513">
         <f>F68+F69+F70</f>
         <v>355407.6199999997</v>
       </c>
-      <c r="L66" s="490"/>
+      <c r="L66" s="514"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
@@ -32693,11 +32693,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="491">
+      <c r="K68" s="515">
         <f>-C4</f>
         <v>-209541.1</v>
       </c>
-      <c r="L68" s="492"/>
+      <c r="L68" s="516"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -32721,22 +32721,22 @@
       <c r="C70" s="119">
         <v>44257</v>
       </c>
-      <c r="D70" s="499" t="s">
+      <c r="D70" s="501" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="500"/>
+      <c r="E70" s="502"/>
       <c r="F70" s="120">
         <v>223014.26</v>
       </c>
-      <c r="I70" s="501" t="s">
+      <c r="I70" s="503" t="s">
         <v>25</v>
       </c>
-      <c r="J70" s="502"/>
-      <c r="K70" s="503">
+      <c r="J70" s="504"/>
+      <c r="K70" s="505">
         <f>K66+K68</f>
         <v>145866.5199999997</v>
       </c>
-      <c r="L70" s="504"/>
+      <c r="L70" s="506"/>
       <c r="P70" s="50"/>
       <c r="Q70" s="7"/>
       <c r="S70" s="121"/>
@@ -32837,6 +32837,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="D65:E65"/>
     <mergeCell ref="P65:Q65"/>
     <mergeCell ref="D66:E66"/>
     <mergeCell ref="I66:J66"/>
@@ -32848,12 +32854,6 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H64:I64"/>
     <mergeCell ref="K64:L64"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="D65:E65"/>
   </mergeCells>
   <phoneticPr fontId="41" type="noConversion"/>
   <pageMargins left="0.51181102362204722" right="0.15748031496062992" top="0.31496062992125984" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -34124,17 +34124,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="506" t="s">
+      <c r="C1" s="487" t="s">
         <v>429</v>
       </c>
-      <c r="D1" s="506"/>
-      <c r="E1" s="506"/>
-      <c r="F1" s="506"/>
-      <c r="G1" s="506"/>
-      <c r="H1" s="506"/>
-      <c r="I1" s="506"/>
-      <c r="J1" s="506"/>
-      <c r="K1" s="506"/>
+      <c r="D1" s="487"/>
+      <c r="E1" s="487"/>
+      <c r="F1" s="487"/>
+      <c r="G1" s="487"/>
+      <c r="H1" s="487"/>
+      <c r="I1" s="487"/>
+      <c r="J1" s="487"/>
+      <c r="K1" s="487"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -34164,17 +34164,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="507" t="s">
+      <c r="B3" s="488" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="508"/>
+      <c r="C3" s="489"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="509" t="s">
+      <c r="H3" s="490" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="509"/>
+      <c r="I3" s="490"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -34203,14 +34203,14 @@
       <c r="D4" s="23">
         <v>44257</v>
       </c>
-      <c r="E4" s="510" t="s">
+      <c r="E4" s="491" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="511"/>
-      <c r="H4" s="512" t="s">
+      <c r="F4" s="492"/>
+      <c r="H4" s="493" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="513"/>
+      <c r="I4" s="494"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -36812,61 +36812,61 @@
       <c r="A62" s="60"/>
       <c r="B62" s="100"/>
       <c r="C62" s="4"/>
-      <c r="H62" s="493" t="s">
+      <c r="H62" s="495" t="s">
         <v>16</v>
       </c>
-      <c r="I62" s="494"/>
+      <c r="I62" s="496"/>
       <c r="J62" s="101"/>
-      <c r="K62" s="495">
+      <c r="K62" s="497">
         <f>I60+L60</f>
         <v>781851.32000000007</v>
       </c>
-      <c r="L62" s="496"/>
-      <c r="M62" s="497">
+      <c r="L62" s="498"/>
+      <c r="M62" s="499">
         <f>M60+N60</f>
         <v>4064802.5</v>
       </c>
-      <c r="N62" s="498"/>
+      <c r="N62" s="500"/>
       <c r="O62" s="102"/>
       <c r="P62" s="99"/>
       <c r="Q62" s="99"/>
       <c r="S62" s="174"/>
     </row>
     <row r="63" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D63" s="505" t="s">
+      <c r="D63" s="507" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="505"/>
+      <c r="E63" s="507"/>
       <c r="F63" s="103">
         <f>F60-K62-C60</f>
         <v>3177878.1399999997</v>
       </c>
       <c r="I63" s="104"/>
       <c r="J63" s="105"/>
-      <c r="P63" s="484">
+      <c r="P63" s="508">
         <f>P60+Q60</f>
         <v>4585432.34</v>
       </c>
-      <c r="Q63" s="485"/>
+      <c r="Q63" s="509"/>
       <c r="S63" s="50"/>
     </row>
     <row r="64" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="486" t="s">
+      <c r="D64" s="510" t="s">
         <v>18</v>
       </c>
-      <c r="E64" s="486"/>
+      <c r="E64" s="510"/>
       <c r="F64" s="95">
         <v>-3579271.89</v>
       </c>
-      <c r="I64" s="487" t="s">
+      <c r="I64" s="511" t="s">
         <v>19</v>
       </c>
-      <c r="J64" s="488"/>
-      <c r="K64" s="489">
+      <c r="J64" s="512"/>
+      <c r="K64" s="513">
         <f>F66+F67+F68</f>
         <v>-110332.85000000047</v>
       </c>
-      <c r="L64" s="490"/>
+      <c r="L64" s="514"/>
       <c r="P64" s="50"/>
       <c r="S64" s="107"/>
     </row>
@@ -36900,11 +36900,11 @@
         <v>21</v>
       </c>
       <c r="J66" s="115"/>
-      <c r="K66" s="491">
+      <c r="K66" s="515">
         <f>-C4</f>
         <v>-223014.26</v>
       </c>
-      <c r="L66" s="492"/>
+      <c r="L66" s="516"/>
       <c r="M66" s="116"/>
       <c r="P66" s="50"/>
       <c r="Q66" s="7"/>
@@ -36928,22 +36928,22 @@
       <c r="C68" s="119">
         <v>44291</v>
       </c>
-      <c r="D68" s="499" t="s">
+      <c r="D68" s="501" t="s">
         <v>24</v>
       </c>
-      <c r="E68" s="500"/>
+      <c r="E68" s="502"/>
       <c r="F68" s="120">
         <v>215362.9</v>
       </c>
-      <c r="I68" s="514" t="s">
+      <c r="I68" s="517" t="s">
         <v>431</v>
       </c>
-      <c r="J68" s="515"/>
-      <c r="K68" s="516">
+      <c r="J68" s="518"/>
+      <c r="K68" s="519">
         <f>K64+K66</f>
         <v>-333347.11000000045</v>
       </c>
-      <c r="L68" s="517"/>
+      <c r="L68" s="520"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
       <c r="S68" s="121"/>
@@ -37099,6 +37099,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="M62:N62"/>
+    <mergeCell ref="D63:E63"/>
     <mergeCell ref="P63:Q63"/>
     <mergeCell ref="D64:E64"/>
     <mergeCell ref="I64:J64"/>
@@ -37110,12 +37116,6 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H62:I62"/>
     <mergeCell ref="K62:L62"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="M62:N62"/>
-    <mergeCell ref="D63:E63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -38547,17 +38547,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="506" t="s">
+      <c r="C1" s="487" t="s">
         <v>430</v>
       </c>
-      <c r="D1" s="506"/>
-      <c r="E1" s="506"/>
-      <c r="F1" s="506"/>
-      <c r="G1" s="506"/>
-      <c r="H1" s="506"/>
-      <c r="I1" s="506"/>
-      <c r="J1" s="506"/>
-      <c r="K1" s="506"/>
+      <c r="D1" s="487"/>
+      <c r="E1" s="487"/>
+      <c r="F1" s="487"/>
+      <c r="G1" s="487"/>
+      <c r="H1" s="487"/>
+      <c r="I1" s="487"/>
+      <c r="J1" s="487"/>
+      <c r="K1" s="487"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -38587,17 +38587,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="507" t="s">
+      <c r="B3" s="488" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="508"/>
+      <c r="C3" s="489"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="509" t="s">
+      <c r="H3" s="490" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="509"/>
+      <c r="I3" s="490"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -38626,14 +38626,14 @@
       <c r="D4" s="23">
         <v>44291</v>
       </c>
-      <c r="E4" s="510" t="s">
+      <c r="E4" s="491" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="511"/>
-      <c r="H4" s="512" t="s">
+      <c r="F4" s="492"/>
+      <c r="H4" s="493" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="519"/>
+      <c r="I4" s="521"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -41125,61 +41125,61 @@
       <c r="A58" s="60"/>
       <c r="B58" s="100"/>
       <c r="C58" s="4"/>
-      <c r="H58" s="493" t="s">
+      <c r="H58" s="495" t="s">
         <v>16</v>
       </c>
-      <c r="I58" s="494"/>
+      <c r="I58" s="496"/>
       <c r="J58" s="101"/>
-      <c r="K58" s="495">
+      <c r="K58" s="497">
         <f>I56+L56</f>
         <v>370346.35000000003</v>
       </c>
-      <c r="L58" s="520"/>
-      <c r="M58" s="497">
+      <c r="L58" s="522"/>
+      <c r="M58" s="499">
         <f>M56+N56</f>
         <v>3537422</v>
       </c>
-      <c r="N58" s="498"/>
+      <c r="N58" s="500"/>
       <c r="O58" s="102"/>
       <c r="P58" s="99"/>
       <c r="Q58" s="99"/>
       <c r="S58" s="174"/>
     </row>
     <row r="59" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="505" t="s">
+      <c r="D59" s="507" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="518"/>
+      <c r="E59" s="523"/>
       <c r="F59" s="103">
         <f>F56-K58-C56</f>
         <v>3048717.54</v>
       </c>
       <c r="I59" s="104"/>
       <c r="J59" s="105"/>
-      <c r="P59" s="484">
+      <c r="P59" s="508">
         <f>P56+Q56</f>
         <v>8073324.3200000003</v>
       </c>
-      <c r="Q59" s="485"/>
+      <c r="Q59" s="509"/>
       <c r="S59" s="50"/>
     </row>
     <row r="60" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D60" s="486" t="s">
+      <c r="D60" s="510" t="s">
         <v>18</v>
       </c>
-      <c r="E60" s="486"/>
+      <c r="E60" s="510"/>
       <c r="F60" s="95">
         <v>-3102716.28</v>
       </c>
-      <c r="I60" s="487" t="s">
+      <c r="I60" s="511" t="s">
         <v>19</v>
       </c>
-      <c r="J60" s="488"/>
-      <c r="K60" s="489">
+      <c r="J60" s="512"/>
+      <c r="K60" s="513">
         <f>F62+F63+F64</f>
         <v>216465.62000000023</v>
       </c>
-      <c r="L60" s="490"/>
+      <c r="L60" s="514"/>
       <c r="P60" s="50"/>
       <c r="S60" s="107"/>
     </row>
@@ -41213,11 +41213,11 @@
         <v>21</v>
       </c>
       <c r="J62" s="115"/>
-      <c r="K62" s="491">
+      <c r="K62" s="515">
         <f>-C4</f>
         <v>-215362.9</v>
       </c>
-      <c r="L62" s="492"/>
+      <c r="L62" s="516"/>
       <c r="M62" s="116"/>
       <c r="P62" s="50"/>
       <c r="Q62" s="7"/>
@@ -41241,22 +41241,22 @@
       <c r="C64" s="119">
         <v>44320</v>
       </c>
-      <c r="D64" s="499" t="s">
+      <c r="D64" s="501" t="s">
         <v>24</v>
       </c>
-      <c r="E64" s="500"/>
+      <c r="E64" s="502"/>
       <c r="F64" s="120">
         <v>249311.35999999999</v>
       </c>
-      <c r="I64" s="501" t="s">
+      <c r="I64" s="503" t="s">
         <v>25</v>
       </c>
-      <c r="J64" s="502"/>
-      <c r="K64" s="503">
+      <c r="J64" s="504"/>
+      <c r="K64" s="505">
         <f>K60+K62</f>
         <v>1102.720000000234</v>
       </c>
-      <c r="L64" s="504"/>
+      <c r="L64" s="506"/>
       <c r="P64" s="50"/>
       <c r="Q64" s="7"/>
       <c r="S64" s="121"/>
@@ -41412,6 +41412,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="I64:J64"/>
+    <mergeCell ref="K64:L64"/>
+    <mergeCell ref="M58:N58"/>
+    <mergeCell ref="D59:E59"/>
     <mergeCell ref="P59:Q59"/>
     <mergeCell ref="D60:E60"/>
     <mergeCell ref="I60:J60"/>
@@ -41423,12 +41429,6 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H58:I58"/>
     <mergeCell ref="K58:L58"/>
-    <mergeCell ref="K62:L62"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="I64:J64"/>
-    <mergeCell ref="K64:L64"/>
-    <mergeCell ref="M58:N58"/>
-    <mergeCell ref="D59:E59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -42311,17 +42311,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="506" t="s">
+      <c r="C1" s="487" t="s">
         <v>504</v>
       </c>
-      <c r="D1" s="506"/>
-      <c r="E1" s="506"/>
-      <c r="F1" s="506"/>
-      <c r="G1" s="506"/>
-      <c r="H1" s="506"/>
-      <c r="I1" s="506"/>
-      <c r="J1" s="506"/>
-      <c r="K1" s="506"/>
+      <c r="D1" s="487"/>
+      <c r="E1" s="487"/>
+      <c r="F1" s="487"/>
+      <c r="G1" s="487"/>
+      <c r="H1" s="487"/>
+      <c r="I1" s="487"/>
+      <c r="J1" s="487"/>
+      <c r="K1" s="487"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -42351,17 +42351,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="507" t="s">
+      <c r="B3" s="488" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="508"/>
+      <c r="C3" s="489"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="509" t="s">
+      <c r="H3" s="490" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="509"/>
+      <c r="I3" s="490"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -42390,14 +42390,14 @@
       <c r="D4" s="23">
         <v>44320</v>
       </c>
-      <c r="E4" s="510" t="s">
+      <c r="E4" s="491" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="511"/>
-      <c r="H4" s="512" t="s">
+      <c r="F4" s="492"/>
+      <c r="H4" s="493" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="513"/>
+      <c r="I4" s="494"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -45274,71 +45274,71 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="493" t="s">
+      <c r="H64" s="495" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="494"/>
+      <c r="I64" s="496"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="495">
+      <c r="K64" s="497">
         <f>I62+L62</f>
         <v>779034.56000000017</v>
       </c>
-      <c r="L64" s="496"/>
-      <c r="M64" s="497">
+      <c r="L64" s="498"/>
+      <c r="M64" s="499">
         <f>M62+N62</f>
         <v>4478181</v>
       </c>
-      <c r="N64" s="498"/>
+      <c r="N64" s="500"/>
       <c r="O64" s="102"/>
       <c r="P64" s="99"/>
       <c r="Q64" s="99"/>
       <c r="S64" s="174"/>
     </row>
     <row r="65" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="505" t="s">
+      <c r="D65" s="507" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="505"/>
+      <c r="E65" s="507"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>3602842.44</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="484">
+      <c r="P65" s="508">
         <f>P62+Q62</f>
         <v>5004562.5599999996</v>
       </c>
-      <c r="Q65" s="485"/>
+      <c r="Q65" s="509"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="521" t="s">
+      <c r="B66" s="524" t="s">
         <v>528</v>
       </c>
-      <c r="C66" s="522"/>
-      <c r="D66" s="505" t="s">
+      <c r="C66" s="525"/>
+      <c r="D66" s="507" t="s">
         <v>502</v>
       </c>
-      <c r="E66" s="505"/>
+      <c r="E66" s="507"/>
       <c r="F66" s="95">
         <v>-3854423.8</v>
       </c>
-      <c r="I66" s="487" t="s">
+      <c r="I66" s="511" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="488"/>
-      <c r="K66" s="489">
+      <c r="J66" s="512"/>
+      <c r="K66" s="513">
         <f>F68+F69+F70</f>
         <v>14998.430000000139</v>
       </c>
-      <c r="L66" s="490"/>
+      <c r="L66" s="514"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
     <row r="67" spans="2:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="523"/>
-      <c r="C67" s="524"/>
+      <c r="B67" s="526"/>
+      <c r="C67" s="527"/>
       <c r="D67" s="108"/>
       <c r="E67" s="60"/>
       <c r="F67" s="109">
@@ -45353,8 +45353,8 @@
       <c r="S67" s="50"/>
     </row>
     <row r="68" spans="2:19" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="525"/>
-      <c r="C68" s="526"/>
+      <c r="B68" s="528"/>
+      <c r="C68" s="529"/>
       <c r="E68" s="60" t="s">
         <v>20</v>
       </c>
@@ -45367,11 +45367,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="491">
+      <c r="K68" s="515">
         <f>-C4</f>
         <v>-249311.35999999999</v>
       </c>
-      <c r="L68" s="492"/>
+      <c r="L68" s="516"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -45395,22 +45395,22 @@
       <c r="C70" s="119">
         <v>44353</v>
       </c>
-      <c r="D70" s="499" t="s">
+      <c r="D70" s="501" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="500"/>
+      <c r="E70" s="502"/>
       <c r="F70" s="120">
         <v>255764.39</v>
       </c>
-      <c r="I70" s="501" t="s">
+      <c r="I70" s="503" t="s">
         <v>431</v>
       </c>
-      <c r="J70" s="502"/>
-      <c r="K70" s="503">
+      <c r="J70" s="504"/>
+      <c r="K70" s="505">
         <f>K66+K68</f>
         <v>-234312.92999999985</v>
       </c>
-      <c r="L70" s="504"/>
+      <c r="L70" s="506"/>
       <c r="P70" s="50"/>
       <c r="Q70" s="7"/>
       <c r="S70" s="121"/>
@@ -45566,6 +45566,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="D65:E65"/>
     <mergeCell ref="P65:Q65"/>
     <mergeCell ref="D66:E66"/>
     <mergeCell ref="I66:J66"/>
@@ -45579,11 +45584,6 @@
     <mergeCell ref="K64:L64"/>
     <mergeCell ref="B66:C68"/>
     <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="D65:E65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>